<commit_message>
updating perennial grain lit
</commit_message>
<xml_diff>
--- a/data/pgrain_literature-summary.xlsx
+++ b/data/pgrain_literature-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\figlib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909262C4-916C-4586-8FD6-7AEBAAD19454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E5D788-D05E-478C-B46E-457EBAAD25BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5490" windowWidth="38640" windowHeight="21120" firstSheet="4" activeTab="11" xr2:uid="{D43F686E-3943-4AA3-B812-49FE601D9B76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="12" xr2:uid="{D43F686E-3943-4AA3-B812-49FE601D9B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Daly_trt_smy" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Jungers2017" sheetId="11" r:id="rId10"/>
     <sheet name="Clark2019" sheetId="12" r:id="rId11"/>
     <sheet name="Bajgain2020" sheetId="13" r:id="rId12"/>
+    <sheet name="Fagnant2024" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="150">
   <si>
     <t>citation</t>
   </si>
@@ -476,6 +477,27 @@
   </si>
   <si>
     <t>Taken from Figure 3 using plot digitizer, only took the highest yielding (MN-Clearwater), it's the mean of several locations though</t>
+  </si>
+  <si>
+    <t>Taken from fig 5 in pub</t>
+  </si>
+  <si>
+    <t>Took all agronomic managements, middle of box distribution (median)</t>
+  </si>
+  <si>
+    <t>Fagnant et al. 2024</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>split application</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Planting density was 250 seeds m-2 while actual plant density was 176 seed m-2</t>
   </si>
 </sst>
 </file>
@@ -1876,7 +1898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C7A390-8787-4ED4-8144-7087C56606E0}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y41" sqref="Y41"/>
     </sheetView>
   </sheetViews>
@@ -1941,6 +1963,236 @@
       </c>
       <c r="F9">
         <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE86612C-AB46-42A0-A02E-62AA41B0820D}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" t="s">
+        <v>135</v>
+      </c>
+      <c r="K6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>590</v>
+      </c>
+      <c r="I7">
+        <v>250</v>
+      </c>
+      <c r="J7">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19">
+        <v>1088</v>
+      </c>
+      <c r="K19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>798</v>
+      </c>
+      <c r="K20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>871</v>
+      </c>
+      <c r="K21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>1022</v>
+      </c>
+      <c r="K22" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -4203,7 +4455,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>